<commit_message>
bayesian model-averaging approach implemented
</commit_message>
<xml_diff>
--- a/codingSheet.xlsx
+++ b/codingSheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanropovik/Library/Mobile Documents/com~apple~CloudDocs/MANUSCRIPTS/ongoing/2020 Cyril Lukas Meta/gamesAttitudesMeta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A532EF3-7DF4-3649-9B55-390BA8354082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB81CA0-B267-A441-BF26-85EDF39A9317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="593" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Coding scheme'!$A$1:$D$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$A$1:$BQ$1</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcMode="manual"/>
+  <calcPr calcId="191029" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7666" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7666" uniqueCount="922">
   <si>
     <t>paperID</t>
   </si>
@@ -2605,9 +2605,6 @@
     <t>game vs passive control</t>
   </si>
   <si>
-    <t>activity related</t>
-  </si>
-  <si>
     <t>activity unrelated</t>
   </si>
   <si>
@@ -2633,9 +2630,6 @@
   </si>
   <si>
     <t>they tried ST-IAT, but itbrought unreliable numbers</t>
-  </si>
-  <si>
-    <t>unrelated activity</t>
   </si>
   <si>
     <t>moorhuhn like shooter game - arousal from the action, not really meaningful, violence is involved though</t>
@@ -3244,9 +3238,6 @@
   </si>
   <si>
     <t>confidential interval between 16-26</t>
-  </si>
-  <si>
-    <t>stereotype rehearsal</t>
   </si>
   <si>
     <t>seExp</t>
@@ -4640,7 +4631,7 @@
         <v>128</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>111</v>
@@ -23028,9 +23019,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BZ143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BL1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BP51" sqref="BP51"/>
+    <sheetView tabSelected="1" topLeftCell="BQ1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BV19" sqref="BV19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23096,7 +23087,7 @@
         <v>14</v>
       </c>
       <c r="Q1" s="24" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="R1" s="24" t="s">
         <v>15</v>
@@ -23144,10 +23135,10 @@
         <v>29</v>
       </c>
       <c r="AG1" s="24" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="AH1" s="24" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="AI1" s="24" t="s">
         <v>30</v>
@@ -23380,7 +23371,7 @@
         <v>320</v>
       </c>
       <c r="AL2" s="26" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="AM2" s="26">
         <v>0</v>
@@ -23407,7 +23398,7 @@
       <c r="AY2" s="26"/>
       <c r="AZ2" s="26"/>
       <c r="BA2" s="26" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="BB2" s="26"/>
       <c r="BC2" s="26">
@@ -23417,7 +23408,7 @@
         <v>702</v>
       </c>
       <c r="BE2" s="26" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="BF2" s="26">
         <v>0</v>
@@ -23574,7 +23565,7 @@
         <v>320</v>
       </c>
       <c r="AL3" s="26" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="AM3" s="26">
         <v>0</v>
@@ -23601,7 +23592,7 @@
       <c r="AY3" s="26"/>
       <c r="AZ3" s="26"/>
       <c r="BA3" s="26" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="BB3" s="26"/>
       <c r="BC3" s="26">
@@ -23611,7 +23602,7 @@
         <v>702</v>
       </c>
       <c r="BE3" s="26" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="BF3" s="26">
         <v>0</v>
@@ -23769,7 +23760,7 @@
         <v>320</v>
       </c>
       <c r="AL4" s="26" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="AM4" s="26">
         <v>0</v>
@@ -23796,7 +23787,7 @@
       <c r="AY4" s="26"/>
       <c r="AZ4" s="26"/>
       <c r="BA4" s="26" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="BB4" s="26"/>
       <c r="BC4" s="26">
@@ -23806,7 +23797,7 @@
         <v>702</v>
       </c>
       <c r="BE4" s="26" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="BF4" s="26">
         <v>365</v>
@@ -23965,7 +23956,7 @@
         <v>320</v>
       </c>
       <c r="AL5" s="26" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="AM5" s="26">
         <v>0</v>
@@ -23992,7 +23983,7 @@
       <c r="AY5" s="30"/>
       <c r="AZ5" s="26"/>
       <c r="BA5" s="26" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="BB5" s="30"/>
       <c r="BC5" s="26">
@@ -24002,7 +23993,7 @@
         <v>702</v>
       </c>
       <c r="BE5" s="26" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="BF5" s="26">
         <v>365</v>
@@ -24213,7 +24204,7 @@
         <v>230</v>
       </c>
       <c r="BL6" s="26" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="BM6" s="26"/>
       <c r="BN6" s="26"/>
@@ -24405,7 +24396,7 @@
         <v>230</v>
       </c>
       <c r="BL7" s="26" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="BM7" s="26"/>
       <c r="BN7" s="26"/>
@@ -24546,10 +24537,10 @@
         <v>725</v>
       </c>
       <c r="AO8" s="31" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="AP8" s="26" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="AQ8" s="26">
         <v>11</v>
@@ -24593,7 +24584,7 @@
         <v>230</v>
       </c>
       <c r="BL8" s="26" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="BM8" s="26"/>
       <c r="BN8" s="26"/>
@@ -24731,13 +24722,13 @@
         <v>1</v>
       </c>
       <c r="AN9" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO9" s="31" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="AP9" s="26" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="AQ9" s="26">
         <v>11</v>
@@ -24781,7 +24772,7 @@
         <v>230</v>
       </c>
       <c r="BL9" s="26" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="BM9" s="26"/>
       <c r="BN9" s="26"/>
@@ -24977,7 +24968,7 @@
         <v>230</v>
       </c>
       <c r="BL10" s="26" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="BM10" s="26"/>
       <c r="BN10" s="26"/>
@@ -27380,7 +27371,7 @@
         <v>0</v>
       </c>
       <c r="M23" s="31" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="N23" s="31" t="s">
         <v>186</v>
@@ -27574,7 +27565,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="31" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="N24" s="34" t="s">
         <v>186</v>
@@ -27768,7 +27759,7 @@
         <v>0</v>
       </c>
       <c r="M25" s="31" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="N25" s="34" t="s">
         <v>186</v>
@@ -27962,7 +27953,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="31" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="N26" s="34" t="s">
         <v>186</v>
@@ -28140,7 +28131,7 @@
         <v>0</v>
       </c>
       <c r="M27" s="31" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="N27" s="34" t="s">
         <v>186</v>
@@ -28207,7 +28198,7 @@
         <v>1</v>
       </c>
       <c r="AN27" s="26" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="AO27" s="26"/>
       <c r="AP27" s="26" t="s">
@@ -28320,7 +28311,7 @@
         <v>0</v>
       </c>
       <c r="M28" s="31" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="N28" s="34" t="s">
         <v>186</v>
@@ -28514,7 +28505,7 @@
         <v>0</v>
       </c>
       <c r="M29" s="31" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="N29" s="34" t="s">
         <v>186</v>
@@ -28708,7 +28699,7 @@
         <v>0</v>
       </c>
       <c r="M30" s="31" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="N30" s="34" t="s">
         <v>655</v>
@@ -28908,7 +28899,7 @@
         <v>0</v>
       </c>
       <c r="M31" s="31" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="N31" s="34" t="s">
         <v>655</v>
@@ -29233,7 +29224,7 @@
         <v>230</v>
       </c>
       <c r="BL32" s="26" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="BM32" s="26"/>
       <c r="BN32" s="26"/>
@@ -29427,7 +29418,7 @@
         <v>230</v>
       </c>
       <c r="BL33" s="26" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="BM33" s="26"/>
       <c r="BN33" s="26"/>
@@ -29496,7 +29487,7 @@
         <v>0</v>
       </c>
       <c r="M34" s="31" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="N34" s="34" t="s">
         <v>617</v>
@@ -32609,10 +32600,10 @@
         <v>1</v>
       </c>
       <c r="M50" s="26" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="N50" s="34" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="O50" s="26" t="s">
         <v>325</v>
@@ -32711,7 +32702,7 @@
         <v>704</v>
       </c>
       <c r="BE50" s="26" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="BF50" s="26">
         <v>0</v>
@@ -32803,10 +32794,10 @@
         <v>1</v>
       </c>
       <c r="M51" s="26" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="N51" s="34" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="O51" s="26" t="s">
         <v>325</v>
@@ -32903,7 +32894,7 @@
         <v>704</v>
       </c>
       <c r="BE51" s="26" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="BF51" s="26">
         <v>28</v>
@@ -33372,7 +33363,7 @@
         <v>344</v>
       </c>
       <c r="N54" s="31" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="O54" s="26" t="s">
         <v>347</v>
@@ -33550,7 +33541,7 @@
         <v>357</v>
       </c>
       <c r="N55" s="31" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="O55" s="34" t="s">
         <v>358</v>
@@ -33646,7 +33637,7 @@
         <v>21</v>
       </c>
       <c r="BD55" s="26" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="BE55" s="31" t="s">
         <v>362</v>
@@ -33742,7 +33733,7 @@
         <v>357</v>
       </c>
       <c r="N56" s="31" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="O56" s="34" t="s">
         <v>358</v>
@@ -33838,7 +33829,7 @@
         <v>21</v>
       </c>
       <c r="BD56" s="26" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="BE56" s="31" t="s">
         <v>362</v>
@@ -33934,7 +33925,7 @@
         <v>357</v>
       </c>
       <c r="N57" s="31" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="O57" s="34" t="s">
         <v>358</v>
@@ -34004,13 +33995,13 @@
         <v>1</v>
       </c>
       <c r="AN57" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO57" s="26" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="AP57" s="26" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="AQ57" s="26">
         <v>2</v>
@@ -34030,7 +34021,7 @@
         <v>21</v>
       </c>
       <c r="BD57" s="26" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="BE57" s="31" t="s">
         <v>362</v>
@@ -34126,7 +34117,7 @@
         <v>357</v>
       </c>
       <c r="N58" s="31" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="O58" s="34" t="s">
         <v>358</v>
@@ -34196,13 +34187,13 @@
         <v>1</v>
       </c>
       <c r="AN58" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO58" s="26" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="AP58" s="26" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="AQ58" s="26">
         <v>2</v>
@@ -34222,7 +34213,7 @@
         <v>21</v>
       </c>
       <c r="BD58" s="26" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="BE58" s="31" t="s">
         <v>362</v>
@@ -34417,7 +34408,7 @@
         <v>128</v>
       </c>
       <c r="BA59" s="26" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="BB59" s="26">
         <v>0.37</v>
@@ -34645,10 +34636,10 @@
         <v>1</v>
       </c>
       <c r="BK60" s="26" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="BL60" s="31" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="BM60" s="31"/>
       <c r="BN60" s="26"/>
@@ -34672,7 +34663,7 @@
         <v>637</v>
       </c>
       <c r="BV60" s="26" t="s">
-        <v>922</v>
+        <v>691</v>
       </c>
       <c r="BW60" s="26">
         <v>1</v>
@@ -34841,10 +34832,10 @@
         <v>1</v>
       </c>
       <c r="BK61" s="26" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="BL61" s="31" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="BM61" s="31"/>
       <c r="BN61" s="26"/>
@@ -34868,7 +34859,7 @@
         <v>637</v>
       </c>
       <c r="BV61" s="26" t="s">
-        <v>922</v>
+        <v>691</v>
       </c>
       <c r="BW61" s="26">
         <v>1</v>
@@ -34916,7 +34907,7 @@
       </c>
       <c r="M62" s="26"/>
       <c r="N62" s="31" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="O62" s="26" t="s">
         <v>382</v>
@@ -35005,7 +34996,7 @@
       <c r="AY62" s="26"/>
       <c r="AZ62" s="26"/>
       <c r="BA62" s="26" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="BB62" s="26">
         <v>0.35</v>
@@ -35104,7 +35095,7 @@
       </c>
       <c r="M63" s="26"/>
       <c r="N63" s="31" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="O63" s="26" t="s">
         <v>382</v>
@@ -35289,10 +35280,10 @@
         <v>0</v>
       </c>
       <c r="M64" s="31" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="N64" s="26" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="O64" s="26" t="s">
         <v>677</v>
@@ -35391,7 +35382,7 @@
         <v>705</v>
       </c>
       <c r="BE64" s="26" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="BF64" s="26">
         <v>0</v>
@@ -35479,7 +35470,7 @@
         <v>0</v>
       </c>
       <c r="M65" s="26" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="N65" s="26"/>
       <c r="O65" s="26" t="s">
@@ -35590,7 +35581,7 @@
         <v>706</v>
       </c>
       <c r="BH65" s="31" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="BI65" s="26" t="s">
         <v>684</v>
@@ -35667,7 +35658,7 @@
         <v>0</v>
       </c>
       <c r="M66" s="26" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="N66" s="26"/>
       <c r="O66" s="26" t="s">
@@ -35738,7 +35729,7 @@
         <v>0</v>
       </c>
       <c r="AN66" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO66" s="31" t="s">
         <v>419</v>
@@ -35788,7 +35779,7 @@
         <v>230</v>
       </c>
       <c r="BL66" s="31" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="BM66" s="31"/>
       <c r="BN66" s="26"/>
@@ -35859,7 +35850,7 @@
         <v>0</v>
       </c>
       <c r="M67" s="26" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="N67" s="26"/>
       <c r="O67" s="26" t="s">
@@ -35930,7 +35921,7 @@
         <v>0</v>
       </c>
       <c r="AN67" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO67" s="31" t="s">
         <v>419</v>
@@ -35980,7 +35971,7 @@
         <v>230</v>
       </c>
       <c r="BL67" s="31" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="BM67" s="31"/>
       <c r="BN67" s="26"/>
@@ -36051,7 +36042,7 @@
         <v>0</v>
       </c>
       <c r="M68" s="26" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="N68" s="26"/>
       <c r="O68" s="26" t="s">
@@ -36122,7 +36113,7 @@
         <v>0</v>
       </c>
       <c r="AN68" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO68" s="31" t="s">
         <v>419</v>
@@ -36172,7 +36163,7 @@
         <v>230</v>
       </c>
       <c r="BL68" s="31" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="BM68" s="31"/>
       <c r="BN68" s="26"/>
@@ -36243,7 +36234,7 @@
         <v>0</v>
       </c>
       <c r="M69" s="26" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="N69" s="26"/>
       <c r="O69" s="26" t="s">
@@ -36314,7 +36305,7 @@
         <v>0</v>
       </c>
       <c r="AN69" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO69" s="31" t="s">
         <v>419</v>
@@ -36364,7 +36355,7 @@
         <v>230</v>
       </c>
       <c r="BL69" s="31" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="BM69" s="31"/>
       <c r="BN69" s="26"/>
@@ -36435,7 +36426,7 @@
         <v>0</v>
       </c>
       <c r="M70" s="26" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="N70" s="26"/>
       <c r="O70" s="26" t="s">
@@ -36506,7 +36497,7 @@
         <v>0</v>
       </c>
       <c r="AN70" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO70" s="31" t="s">
         <v>419</v>
@@ -36556,7 +36547,7 @@
         <v>230</v>
       </c>
       <c r="BL70" s="31" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="BM70" s="31"/>
       <c r="BN70" s="26"/>
@@ -36627,7 +36618,7 @@
         <v>0</v>
       </c>
       <c r="M71" s="26" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="N71" s="26"/>
       <c r="O71" s="26" t="s">
@@ -36698,7 +36689,7 @@
         <v>0</v>
       </c>
       <c r="AN71" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO71" s="31" t="s">
         <v>419</v>
@@ -36748,7 +36739,7 @@
         <v>230</v>
       </c>
       <c r="BL71" s="31" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="BM71" s="31"/>
       <c r="BN71" s="26"/>
@@ -36893,7 +36884,7 @@
         <v>318</v>
       </c>
       <c r="AO72" s="26" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="AP72" s="26" t="s">
         <v>302</v>
@@ -37066,7 +37057,7 @@
         <v>1</v>
       </c>
       <c r="AN73" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO73" s="26" t="s">
         <v>453</v>
@@ -37144,7 +37135,7 @@
         <v>0</v>
       </c>
       <c r="BX73" s="26" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
     </row>
     <row r="74" spans="1:76" ht="102" x14ac:dyDescent="0.2">
@@ -37238,7 +37229,7 @@
         <v>1</v>
       </c>
       <c r="AN74" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AO74" s="26" t="s">
         <v>461</v>
@@ -37316,7 +37307,7 @@
         <v>0</v>
       </c>
       <c r="BX74" s="26" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
     </row>
     <row r="75" spans="1:76" ht="51" x14ac:dyDescent="0.2">
@@ -37355,7 +37346,7 @@
         <v>1</v>
       </c>
       <c r="M75" s="26" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="N75" s="26"/>
       <c r="O75" s="26" t="s">
@@ -37428,7 +37419,7 @@
         <v>1</v>
       </c>
       <c r="AN75" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO75" s="26" t="s">
         <v>466</v>
@@ -37457,7 +37448,7 @@
         <v>703</v>
       </c>
       <c r="BE75" s="26" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="BF75" s="26">
         <v>0</v>
@@ -37617,7 +37608,7 @@
         <v>1</v>
       </c>
       <c r="AN76" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO76" s="26" t="s">
         <v>478</v>
@@ -37808,7 +37799,7 @@
         <v>1</v>
       </c>
       <c r="AN77" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO77" s="26" t="s">
         <v>478</v>
@@ -38001,7 +37992,7 @@
         <v>1</v>
       </c>
       <c r="AN78" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO78" s="26" t="s">
         <v>478</v>
@@ -38194,7 +38185,7 @@
         <v>1</v>
       </c>
       <c r="AN79" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO79" s="26" t="s">
         <v>478</v>
@@ -38387,7 +38378,7 @@
         <v>1</v>
       </c>
       <c r="AN80" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO80" s="26" t="s">
         <v>478</v>
@@ -38580,7 +38571,7 @@
         <v>1</v>
       </c>
       <c r="AN81" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO81" s="26" t="s">
         <v>478</v>
@@ -38773,7 +38764,7 @@
         <v>1</v>
       </c>
       <c r="AN82" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO82" s="26" t="s">
         <v>478</v>
@@ -38966,7 +38957,7 @@
         <v>1</v>
       </c>
       <c r="AN83" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO83" s="26" t="s">
         <v>478</v>
@@ -39159,7 +39150,7 @@
         <v>1</v>
       </c>
       <c r="AN84" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO84" s="26" t="s">
         <v>478</v>
@@ -39352,7 +39343,7 @@
         <v>1</v>
       </c>
       <c r="AN85" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO85" s="26" t="s">
         <v>478</v>
@@ -39545,7 +39536,7 @@
         <v>1</v>
       </c>
       <c r="AN86" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO86" s="26" t="s">
         <v>478</v>
@@ -39738,7 +39729,7 @@
         <v>1</v>
       </c>
       <c r="AN87" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO87" s="26" t="s">
         <v>478</v>
@@ -39861,7 +39852,7 @@
         <v>1</v>
       </c>
       <c r="M88" s="26" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="N88" s="26" t="s">
         <v>507</v>
@@ -39931,7 +39922,7 @@
         <v>0</v>
       </c>
       <c r="AN88" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AO88" s="26" t="s">
         <v>505</v>
@@ -40052,7 +40043,7 @@
         <v>1</v>
       </c>
       <c r="M89" s="26" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="N89" s="26"/>
       <c r="O89" s="26" t="s">
@@ -40120,7 +40111,7 @@
         <v>0</v>
       </c>
       <c r="AN89" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AO89" s="26" t="s">
         <v>505</v>
@@ -40241,7 +40232,7 @@
         <v>1</v>
       </c>
       <c r="M90" s="26" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="N90" s="26" t="s">
         <v>507</v>
@@ -40311,7 +40302,7 @@
         <v>0</v>
       </c>
       <c r="AN90" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AO90" s="26" t="s">
         <v>505</v>
@@ -40432,7 +40423,7 @@
         <v>1</v>
       </c>
       <c r="M91" s="26" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="N91" s="26" t="s">
         <v>512</v>
@@ -40502,7 +40493,7 @@
         <v>0</v>
       </c>
       <c r="AN91" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AO91" s="26" t="s">
         <v>505</v>
@@ -40623,7 +40614,7 @@
         <v>1</v>
       </c>
       <c r="M92" s="26" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="N92" s="26" t="s">
         <v>507</v>
@@ -40693,7 +40684,7 @@
         <v>0</v>
       </c>
       <c r="AN92" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AO92" s="26" t="s">
         <v>505</v>
@@ -40814,7 +40805,7 @@
         <v>1</v>
       </c>
       <c r="M93" s="26" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="N93" s="26"/>
       <c r="O93" s="26" t="s">
@@ -40882,7 +40873,7 @@
         <v>0</v>
       </c>
       <c r="AN93" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AO93" s="26" t="s">
         <v>505</v>
@@ -41003,7 +40994,7 @@
         <v>1</v>
       </c>
       <c r="M94" s="26" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="N94" s="26" t="s">
         <v>507</v>
@@ -41073,7 +41064,7 @@
         <v>0</v>
       </c>
       <c r="AN94" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AO94" s="26" t="s">
         <v>505</v>
@@ -41194,7 +41185,7 @@
         <v>1</v>
       </c>
       <c r="M95" s="26" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="N95" s="26"/>
       <c r="O95" s="26" t="s">
@@ -41260,7 +41251,7 @@
         <v>0</v>
       </c>
       <c r="AN95" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AO95" s="26" t="s">
         <v>505</v>
@@ -41436,13 +41427,13 @@
         <v>320</v>
       </c>
       <c r="AL96" s="26" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="AM96" s="26">
         <v>0</v>
       </c>
       <c r="AN96" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AO96" s="26" t="s">
         <v>505</v>
@@ -41561,7 +41552,7 @@
         <v>1</v>
       </c>
       <c r="M97" s="26" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="N97" s="26" t="s">
         <v>656</v>
@@ -41618,13 +41609,13 @@
         <v>320</v>
       </c>
       <c r="AL97" s="26" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="AM97" s="26">
         <v>0</v>
       </c>
       <c r="AN97" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AO97" s="26" t="s">
         <v>505</v>
@@ -41800,13 +41791,13 @@
         <v>320</v>
       </c>
       <c r="AL98" s="26" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="AM98" s="26">
         <v>0</v>
       </c>
       <c r="AN98" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AO98" s="26" t="s">
         <v>505</v>
@@ -41982,13 +41973,13 @@
         <v>320</v>
       </c>
       <c r="AL99" s="26" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="AM99" s="26">
         <v>0</v>
       </c>
       <c r="AN99" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AO99" s="26" t="s">
         <v>505</v>
@@ -42108,10 +42099,10 @@
       </c>
       <c r="M100" s="26"/>
       <c r="N100" s="26" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="O100" s="26" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="P100" s="26" t="s">
         <v>132</v>
@@ -42166,19 +42157,19 @@
         <v>320</v>
       </c>
       <c r="AL100" s="26" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="AM100" s="26">
         <v>1</v>
       </c>
       <c r="AN100" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO100" s="26" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="AP100" s="26" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="AQ100" s="26">
         <v>1</v>
@@ -42234,10 +42225,10 @@
         <v>1</v>
       </c>
       <c r="BR100" s="31" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="BS100" s="31" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="BT100" s="26">
         <v>1</v>
@@ -42292,10 +42283,10 @@
       </c>
       <c r="M101" s="26"/>
       <c r="N101" s="26" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="O101" s="26" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="P101" s="26" t="s">
         <v>132</v>
@@ -42350,19 +42341,19 @@
         <v>320</v>
       </c>
       <c r="AL101" s="26" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="AM101" s="26">
         <v>1</v>
       </c>
       <c r="AN101" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO101" s="26" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="AP101" s="26" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="AQ101" s="26">
         <v>1</v>
@@ -42418,10 +42409,10 @@
         <v>1</v>
       </c>
       <c r="BR101" s="31" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="BS101" s="31" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="BT101" s="26">
         <v>1</v>
@@ -43574,7 +43565,9 @@
       <c r="V108" s="26">
         <v>1</v>
       </c>
-      <c r="W108" s="26"/>
+      <c r="W108" s="26">
+        <v>1</v>
+      </c>
       <c r="X108" s="26">
         <v>148</v>
       </c>
@@ -43606,7 +43599,7 @@
         <v>1</v>
       </c>
       <c r="AN108" s="26" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="AO108" s="26" t="s">
         <v>542</v>
@@ -43788,13 +43781,13 @@
         <v>1</v>
       </c>
       <c r="AN109" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO109" s="26" t="s">
+        <v>732</v>
+      </c>
+      <c r="AP109" s="26" t="s">
         <v>733</v>
-      </c>
-      <c r="AP109" s="26" t="s">
-        <v>734</v>
       </c>
       <c r="AQ109" s="26">
         <v>9</v>
@@ -43826,7 +43819,7 @@
         <v>705</v>
       </c>
       <c r="BH109" s="26" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="BI109" s="26" t="s">
         <v>684</v>
@@ -43965,7 +43958,7 @@
         <v>318</v>
       </c>
       <c r="AO110" s="26" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="AP110" s="26" t="s">
         <v>302</v>
@@ -44000,7 +43993,7 @@
         <v>705</v>
       </c>
       <c r="BH110" s="26" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="BI110" s="26" t="s">
         <v>684</v>
@@ -44081,7 +44074,7 @@
         <v>1</v>
       </c>
       <c r="M111" s="26" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="N111" s="31" t="s">
         <v>569</v>
@@ -44156,7 +44149,7 @@
         <v>1</v>
       </c>
       <c r="AN111" s="26" t="s">
-        <v>739</v>
+        <v>721</v>
       </c>
       <c r="AO111" s="31" t="s">
         <v>567</v>
@@ -44202,7 +44195,7 @@
         <v>251</v>
       </c>
       <c r="BN111" s="26" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="BO111" s="26" t="s">
         <v>564</v>
@@ -44223,7 +44216,7 @@
         <v>2</v>
       </c>
       <c r="BU111" s="26" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="BV111" s="26" t="s">
         <v>692</v>
@@ -44273,7 +44266,7 @@
         <v>1</v>
       </c>
       <c r="M112" s="26" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="N112" s="31" t="s">
         <v>571</v>
@@ -44348,13 +44341,13 @@
         <v>1</v>
       </c>
       <c r="AN112" s="26" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="AO112" s="31" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="AP112" s="26" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="AQ112" s="26"/>
       <c r="AR112" s="26"/>
@@ -44394,7 +44387,7 @@
         <v>251</v>
       </c>
       <c r="BN112" s="26" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="BO112" s="26" t="s">
         <v>564</v>
@@ -44415,7 +44408,7 @@
         <v>2</v>
       </c>
       <c r="BU112" s="26" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="BV112" s="26"/>
       <c r="BW112" s="26">
@@ -44463,7 +44456,7 @@
         <v>1</v>
       </c>
       <c r="M113" s="26" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="N113" s="31" t="s">
         <v>571</v>
@@ -44538,13 +44531,13 @@
         <v>1</v>
       </c>
       <c r="AN113" s="26" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="AO113" s="31" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="AP113" s="26" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="AQ113" s="26"/>
       <c r="AR113" s="26"/>
@@ -44584,7 +44577,7 @@
         <v>251</v>
       </c>
       <c r="BN113" s="26" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="BO113" s="26" t="s">
         <v>564</v>
@@ -44605,7 +44598,7 @@
         <v>2</v>
       </c>
       <c r="BU113" s="26" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="BV113" s="26"/>
       <c r="BW113" s="26">
@@ -44720,7 +44713,7 @@
         <v>1</v>
       </c>
       <c r="AN114" s="26" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="AO114" s="31" t="s">
         <v>581</v>
@@ -44914,7 +44907,7 @@
         <v>0</v>
       </c>
       <c r="AN115" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AO115" s="26" t="s">
         <v>505</v>
@@ -45110,7 +45103,7 @@
         <v>0</v>
       </c>
       <c r="AN116" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AO116" s="26" t="s">
         <v>505</v>
@@ -45306,7 +45299,7 @@
         <v>0</v>
       </c>
       <c r="AN117" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AO117" s="26" t="s">
         <v>505</v>
@@ -45502,7 +45495,7 @@
         <v>0</v>
       </c>
       <c r="AN118" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AO118" s="26" t="s">
         <v>505</v>
@@ -45698,7 +45691,7 @@
         <v>0</v>
       </c>
       <c r="AN119" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AO119" s="26" t="s">
         <v>505</v>
@@ -45894,7 +45887,7 @@
         <v>0</v>
       </c>
       <c r="AN120" s="26" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="AO120" s="26" t="s">
         <v>505</v>
@@ -46214,13 +46207,13 @@
         <v>609</v>
       </c>
       <c r="N122" s="26" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="O122" s="26" t="s">
         <v>192</v>
       </c>
       <c r="P122" s="34" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="Q122" s="34">
         <v>4</v>
@@ -46278,10 +46271,10 @@
         <v>1</v>
       </c>
       <c r="AN122" s="26" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="AO122" s="26" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="AP122" s="26" t="s">
         <v>407</v>
@@ -46407,7 +46400,7 @@
         <v>1</v>
       </c>
       <c r="M123" s="26" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="N123" s="26"/>
       <c r="O123" s="26" t="s">
@@ -46589,7 +46582,7 @@
         <v>1</v>
       </c>
       <c r="M124" s="26" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="N124" s="26"/>
       <c r="O124" s="26" t="s">
@@ -46650,10 +46643,10 @@
         <v>1</v>
       </c>
       <c r="AN124" s="26" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="AO124" s="26" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="AP124" s="26" t="s">
         <v>407</v>
@@ -46749,7 +46742,7 @@
         <v>662</v>
       </c>
       <c r="E125" s="33" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="F125" s="31" t="s">
         <v>661</v>
@@ -46838,7 +46831,7 @@
         <v>1</v>
       </c>
       <c r="AN125" s="26" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="AO125" s="26" t="s">
         <v>666</v>
@@ -46935,7 +46928,7 @@
         <v>662</v>
       </c>
       <c r="E126" s="33" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="F126" s="31" t="s">
         <v>661</v>
@@ -47024,7 +47017,7 @@
         <v>1</v>
       </c>
       <c r="AN126" s="26" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="AO126" s="26" t="s">
         <v>666</v>
@@ -47123,7 +47116,7 @@
         <v>662</v>
       </c>
       <c r="E127" s="33" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="F127" s="31" t="s">
         <v>661</v>
@@ -47212,7 +47205,7 @@
         <v>1</v>
       </c>
       <c r="AN127" s="26" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="AO127" s="26" t="s">
         <v>666</v>
@@ -47309,7 +47302,7 @@
         <v>662</v>
       </c>
       <c r="E128" s="33" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="F128" s="31" t="s">
         <v>661</v>
@@ -47398,7 +47391,7 @@
         <v>1</v>
       </c>
       <c r="AN128" s="26" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="AO128" s="26" t="s">
         <v>666</v>
@@ -47497,7 +47490,7 @@
         <v>662</v>
       </c>
       <c r="E129" s="33" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="F129" s="31" t="s">
         <v>661</v>
@@ -47586,7 +47579,7 @@
         <v>1</v>
       </c>
       <c r="AN129" s="26" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="AO129" s="26" t="s">
         <v>666</v>
@@ -47683,7 +47676,7 @@
         <v>662</v>
       </c>
       <c r="E130" s="33" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="F130" s="31" t="s">
         <v>661</v>
@@ -47772,7 +47765,7 @@
         <v>1</v>
       </c>
       <c r="AN130" s="26" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="AO130" s="26" t="s">
         <v>666</v>
@@ -47868,13 +47861,13 @@
         <v>1</v>
       </c>
       <c r="D131" s="27" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="E131" s="26" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="F131" s="31" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="G131" s="26">
         <v>2019</v>
@@ -47895,7 +47888,7 @@
       <c r="M131" s="26"/>
       <c r="N131" s="26"/>
       <c r="O131" s="26" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="P131" s="26"/>
       <c r="Q131" s="26">
@@ -47956,7 +47949,7 @@
         <v>320</v>
       </c>
       <c r="AL131" s="31" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="AM131" s="26">
         <v>1</v>
@@ -47997,7 +47990,7 @@
       </c>
       <c r="BH131" s="26"/>
       <c r="BI131" s="26" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="BJ131" s="26">
         <v>0</v>
@@ -48018,7 +48011,7 @@
         <v>0</v>
       </c>
       <c r="BR131" s="26" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="BS131" s="26" t="s">
         <v>644</v>
@@ -48048,13 +48041,13 @@
         <v>1</v>
       </c>
       <c r="D132" s="27" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="E132" s="26" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="F132" s="31" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="G132" s="26">
         <v>2019</v>
@@ -48075,7 +48068,7 @@
       <c r="M132" s="26"/>
       <c r="N132" s="26"/>
       <c r="O132" s="26" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="P132" s="26"/>
       <c r="Q132" s="26">
@@ -48136,7 +48129,7 @@
         <v>320</v>
       </c>
       <c r="AL132" s="31" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="AM132" s="26">
         <v>1</v>
@@ -48145,7 +48138,7 @@
         <v>724</v>
       </c>
       <c r="AO132" s="26" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="AP132" s="26" t="s">
         <v>541</v>
@@ -48185,7 +48178,7 @@
       </c>
       <c r="BH132" s="26"/>
       <c r="BI132" s="26" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="BJ132" s="26">
         <v>0</v>
@@ -48236,13 +48229,13 @@
         <v>1</v>
       </c>
       <c r="D133" s="27" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="E133" s="26" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="F133" s="31" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="G133" s="26">
         <v>2006</v>
@@ -48261,13 +48254,13 @@
         <v>0</v>
       </c>
       <c r="M133" s="26" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="N133" s="26" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="O133" s="26" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="P133" s="26"/>
       <c r="Q133" s="26">
@@ -48328,7 +48321,7 @@
         <v>320</v>
       </c>
       <c r="AL133" s="26" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="AM133" s="26">
         <v>1</v>
@@ -48337,10 +48330,10 @@
         <v>724</v>
       </c>
       <c r="AO133" s="26" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="AP133" s="26" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="AQ133" s="26"/>
       <c r="AR133" s="26"/>
@@ -48369,16 +48362,16 @@
       </c>
       <c r="BH133" s="26"/>
       <c r="BI133" s="26" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="BJ133" s="26">
         <v>1</v>
       </c>
       <c r="BK133" s="26" t="s">
+        <v>809</v>
+      </c>
+      <c r="BL133" s="26" t="s">
         <v>811</v>
-      </c>
-      <c r="BL133" s="26" t="s">
-        <v>813</v>
       </c>
       <c r="BM133" s="26"/>
       <c r="BN133" s="26"/>
@@ -48404,7 +48397,7 @@
         <v>1</v>
       </c>
       <c r="BV133" s="26" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="BW133" s="26">
         <v>1</v>
@@ -48424,13 +48417,13 @@
         <v>2</v>
       </c>
       <c r="D134" s="27" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="E134" s="26" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="F134" s="31" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="G134" s="26">
         <v>2006</v>
@@ -48449,13 +48442,13 @@
         <v>0</v>
       </c>
       <c r="M134" s="26" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="N134" s="26" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="O134" s="26" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="P134" s="26"/>
       <c r="Q134" s="26">
@@ -48516,7 +48509,7 @@
         <v>320</v>
       </c>
       <c r="AL134" s="26" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="AM134" s="26">
         <v>1</v>
@@ -48525,10 +48518,10 @@
         <v>724</v>
       </c>
       <c r="AO134" s="26" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="AP134" s="26" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="AQ134" s="26"/>
       <c r="AR134" s="26"/>
@@ -48557,16 +48550,16 @@
       </c>
       <c r="BH134" s="26"/>
       <c r="BI134" s="26" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="BJ134" s="26">
         <v>1</v>
       </c>
       <c r="BK134" s="26" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="BL134" s="26" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="BM134" s="26"/>
       <c r="BN134" s="26"/>
@@ -48592,7 +48585,7 @@
         <v>1</v>
       </c>
       <c r="BV134" s="26" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="BW134" s="26">
         <v>1</v>
@@ -48612,13 +48605,13 @@
         <v>3</v>
       </c>
       <c r="D135" s="27" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="E135" s="26" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="F135" s="31" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="G135" s="26">
         <v>2006</v>
@@ -48637,13 +48630,13 @@
         <v>0</v>
       </c>
       <c r="M135" s="26" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="N135" s="26" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="O135" s="26" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="P135" s="26"/>
       <c r="Q135" s="26">
@@ -48704,7 +48697,7 @@
         <v>320</v>
       </c>
       <c r="AL135" s="26" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="AM135" s="26">
         <v>1</v>
@@ -48713,10 +48706,10 @@
         <v>724</v>
       </c>
       <c r="AO135" s="26" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="AP135" s="26" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="AQ135" s="26"/>
       <c r="AR135" s="26"/>
@@ -48745,16 +48738,16 @@
       </c>
       <c r="BH135" s="26"/>
       <c r="BI135" s="26" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="BJ135" s="26">
         <v>1</v>
       </c>
       <c r="BK135" s="26" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="BL135" s="26" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="BM135" s="26"/>
       <c r="BN135" s="26"/>
@@ -48780,7 +48773,7 @@
         <v>1</v>
       </c>
       <c r="BV135" s="26" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="BW135" s="26">
         <v>1</v>
@@ -48800,13 +48793,13 @@
         <v>4</v>
       </c>
       <c r="D136" s="27" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="E136" s="26" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="F136" s="31" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="G136" s="26">
         <v>2006</v>
@@ -48825,13 +48818,13 @@
         <v>0</v>
       </c>
       <c r="M136" s="26" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="N136" s="26" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="O136" s="26" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="P136" s="26"/>
       <c r="Q136" s="26">
@@ -48892,7 +48885,7 @@
         <v>320</v>
       </c>
       <c r="AL136" s="26" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="AM136" s="26">
         <v>1</v>
@@ -48901,10 +48894,10 @@
         <v>724</v>
       </c>
       <c r="AO136" s="26" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="AP136" s="26" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="AQ136" s="26"/>
       <c r="AR136" s="26"/>
@@ -48933,16 +48926,16 @@
       </c>
       <c r="BH136" s="26"/>
       <c r="BI136" s="26" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="BJ136" s="26">
         <v>1</v>
       </c>
       <c r="BK136" s="26" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="BL136" s="26" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="BM136" s="26"/>
       <c r="BN136" s="26"/>
@@ -48968,7 +48961,7 @@
         <v>1</v>
       </c>
       <c r="BV136" s="26" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="BW136" s="26">
         <v>1</v>
@@ -48988,13 +48981,13 @@
         <v>5</v>
       </c>
       <c r="D137" s="27" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="E137" s="26" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="F137" s="31" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="G137" s="26">
         <v>2006</v>
@@ -49013,13 +49006,13 @@
         <v>0</v>
       </c>
       <c r="M137" s="26" t="s">
+        <v>813</v>
+      </c>
+      <c r="N137" s="26" t="s">
         <v>815</v>
       </c>
-      <c r="N137" s="26" t="s">
-        <v>817</v>
-      </c>
       <c r="O137" s="26" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="P137" s="26"/>
       <c r="Q137" s="26">
@@ -49080,7 +49073,7 @@
         <v>320</v>
       </c>
       <c r="AL137" s="26" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="AM137" s="26">
         <v>1</v>
@@ -49089,10 +49082,10 @@
         <v>724</v>
       </c>
       <c r="AO137" s="26" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="AP137" s="26" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="AQ137" s="26"/>
       <c r="AR137" s="26"/>
@@ -49121,16 +49114,16 @@
       </c>
       <c r="BH137" s="26"/>
       <c r="BI137" s="26" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="BJ137" s="26">
         <v>1</v>
       </c>
       <c r="BK137" s="26" t="s">
+        <v>809</v>
+      </c>
+      <c r="BL137" s="26" t="s">
         <v>811</v>
-      </c>
-      <c r="BL137" s="26" t="s">
-        <v>813</v>
       </c>
       <c r="BM137" s="26"/>
       <c r="BN137" s="26"/>
@@ -49156,7 +49149,7 @@
         <v>1</v>
       </c>
       <c r="BV137" s="26" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="BW137" s="26">
         <v>1</v>
@@ -49176,13 +49169,13 @@
         <v>6</v>
       </c>
       <c r="D138" s="27" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="E138" s="26" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="F138" s="31" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="G138" s="26">
         <v>2006</v>
@@ -49201,13 +49194,13 @@
         <v>0</v>
       </c>
       <c r="M138" s="26" t="s">
+        <v>813</v>
+      </c>
+      <c r="N138" s="26" t="s">
         <v>815</v>
       </c>
-      <c r="N138" s="26" t="s">
-        <v>817</v>
-      </c>
       <c r="O138" s="26" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="P138" s="26"/>
       <c r="Q138" s="26">
@@ -49268,7 +49261,7 @@
         <v>320</v>
       </c>
       <c r="AL138" s="26" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="AM138" s="26">
         <v>1</v>
@@ -49277,10 +49270,10 @@
         <v>724</v>
       </c>
       <c r="AO138" s="26" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="AP138" s="26" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="AQ138" s="26"/>
       <c r="AR138" s="26"/>
@@ -49309,16 +49302,16 @@
       </c>
       <c r="BH138" s="26"/>
       <c r="BI138" s="26" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="BJ138" s="26">
         <v>1</v>
       </c>
       <c r="BK138" s="26" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="BL138" s="26" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="BM138" s="26"/>
       <c r="BN138" s="26"/>
@@ -49344,7 +49337,7 @@
         <v>1</v>
       </c>
       <c r="BV138" s="26" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="BW138" s="26">
         <v>1</v>
@@ -49364,13 +49357,13 @@
         <v>7</v>
       </c>
       <c r="D139" s="27" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="E139" s="26" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="F139" s="31" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="G139" s="26">
         <v>2006</v>
@@ -49389,13 +49382,13 @@
         <v>0</v>
       </c>
       <c r="M139" s="26" t="s">
+        <v>813</v>
+      </c>
+      <c r="N139" s="26" t="s">
         <v>815</v>
       </c>
-      <c r="N139" s="26" t="s">
-        <v>817</v>
-      </c>
       <c r="O139" s="26" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="P139" s="26"/>
       <c r="Q139" s="26">
@@ -49456,7 +49449,7 @@
         <v>320</v>
       </c>
       <c r="AL139" s="26" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="AM139" s="26">
         <v>1</v>
@@ -49465,10 +49458,10 @@
         <v>724</v>
       </c>
       <c r="AO139" s="26" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="AP139" s="26" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="AQ139" s="26"/>
       <c r="AR139" s="26"/>
@@ -49497,16 +49490,16 @@
       </c>
       <c r="BH139" s="26"/>
       <c r="BI139" s="26" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="BJ139" s="26">
         <v>1</v>
       </c>
       <c r="BK139" s="26" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="BL139" s="26" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="BM139" s="26"/>
       <c r="BN139" s="26"/>
@@ -49532,7 +49525,7 @@
         <v>1</v>
       </c>
       <c r="BV139" s="26" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="BW139" s="26">
         <v>1</v>
@@ -49552,13 +49545,13 @@
         <v>8</v>
       </c>
       <c r="D140" s="27" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="E140" s="26" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="F140" s="31" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="G140" s="26">
         <v>2006</v>
@@ -49577,13 +49570,13 @@
         <v>0</v>
       </c>
       <c r="M140" s="26" t="s">
+        <v>813</v>
+      </c>
+      <c r="N140" s="26" t="s">
         <v>815</v>
       </c>
-      <c r="N140" s="26" t="s">
-        <v>817</v>
-      </c>
       <c r="O140" s="26" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="P140" s="26"/>
       <c r="Q140" s="26">
@@ -49644,7 +49637,7 @@
         <v>320</v>
       </c>
       <c r="AL140" s="26" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="AM140" s="26">
         <v>1</v>
@@ -49653,10 +49646,10 @@
         <v>724</v>
       </c>
       <c r="AO140" s="26" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="AP140" s="26" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="AQ140" s="26"/>
       <c r="AR140" s="26"/>
@@ -49685,16 +49678,16 @@
       </c>
       <c r="BH140" s="26"/>
       <c r="BI140" s="26" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="BJ140" s="26">
         <v>1</v>
       </c>
       <c r="BK140" s="26" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="BL140" s="26" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="BM140" s="26"/>
       <c r="BN140" s="26"/>
@@ -49720,7 +49713,7 @@
         <v>1</v>
       </c>
       <c r="BV140" s="26" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="BW140" s="26">
         <v>1</v>
@@ -49741,10 +49734,10 @@
       </c>
       <c r="D141" s="26"/>
       <c r="E141" s="26" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="F141" s="31" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="G141" s="26">
         <v>2009</v>
@@ -49764,10 +49757,10 @@
       </c>
       <c r="M141" s="26"/>
       <c r="N141" s="26" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="O141" s="26" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="P141" s="26"/>
       <c r="Q141" s="26">
@@ -49814,19 +49807,19 @@
         <v>320</v>
       </c>
       <c r="AL141" s="31" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="AM141" s="26">
         <v>1</v>
       </c>
       <c r="AN141" s="26" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="AO141" s="26" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="AP141" s="26" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="AQ141" s="26"/>
       <c r="AR141" s="26">
@@ -49863,7 +49856,7 @@
         <v>0</v>
       </c>
       <c r="BI141" s="26" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="BJ141" s="26">
         <v>0</v>
@@ -49875,7 +49868,7 @@
       </c>
       <c r="BN141" s="26"/>
       <c r="BO141" s="26" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="BP141" s="26">
         <v>1</v>
@@ -49893,7 +49886,7 @@
         <v>2</v>
       </c>
       <c r="BU141" s="26" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="BV141" s="26" t="s">
         <v>691</v>
@@ -49916,13 +49909,13 @@
         <v>1</v>
       </c>
       <c r="D142" s="27" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="E142" s="33" t="s">
         <v>323</v>
       </c>
       <c r="F142" s="31" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="G142" s="26">
         <v>2020</v>
@@ -49943,10 +49936,10 @@
         <v>1</v>
       </c>
       <c r="M142" s="26" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="N142" s="26" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="O142" s="26" t="s">
         <v>325</v>
@@ -50012,7 +50005,7 @@
         <v>320</v>
       </c>
       <c r="AL142" s="31" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="AM142" s="26">
         <v>1</v>
@@ -50021,10 +50014,10 @@
         <v>724</v>
       </c>
       <c r="AO142" s="31" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="AP142" s="26" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="AQ142" s="26">
         <v>16</v>
@@ -50047,7 +50040,7 @@
         <v>703</v>
       </c>
       <c r="BE142" s="26" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="BF142" s="26">
         <v>0</v>
@@ -50059,19 +50052,19 @@
         <v>0</v>
       </c>
       <c r="BI142" s="26" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="BJ142" s="26">
         <v>1</v>
       </c>
       <c r="BK142" s="31" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="BL142" s="26"/>
       <c r="BM142" s="26"/>
       <c r="BN142" s="26"/>
       <c r="BO142" s="26" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="BP142" s="26">
         <v>1</v>
@@ -50092,7 +50085,7 @@
         <v>1</v>
       </c>
       <c r="BV142" s="26" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="BW142" s="26"/>
       <c r="BX142" s="26" t="s">
@@ -50110,13 +50103,13 @@
         <v>2</v>
       </c>
       <c r="D143" s="27" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="E143" s="33" t="s">
         <v>323</v>
       </c>
       <c r="F143" s="31" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="G143" s="26">
         <v>2020</v>
@@ -50137,10 +50130,10 @@
         <v>1</v>
       </c>
       <c r="M143" s="26" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="N143" s="26" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="O143" s="26" t="s">
         <v>325</v>
@@ -50206,7 +50199,7 @@
         <v>320</v>
       </c>
       <c r="AL143" s="31" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="AM143" s="26">
         <v>1</v>
@@ -50215,10 +50208,10 @@
         <v>724</v>
       </c>
       <c r="AO143" s="31" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="AP143" s="26" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="AQ143" s="26">
         <v>16</v>
@@ -50241,7 +50234,7 @@
         <v>703</v>
       </c>
       <c r="BE143" s="26" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="BF143" s="26">
         <v>28</v>
@@ -50250,22 +50243,22 @@
         <v>706</v>
       </c>
       <c r="BH143" s="37" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="BI143" s="26" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="BJ143" s="26">
         <v>1</v>
       </c>
       <c r="BK143" s="31" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="BL143" s="26"/>
       <c r="BM143" s="26"/>
       <c r="BN143" s="26"/>
       <c r="BO143" s="26" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="BP143" s="26">
         <v>1</v>
@@ -50286,7 +50279,7 @@
         <v>1</v>
       </c>
       <c r="BV143" s="26" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="BW143" s="26"/>
       <c r="BX143" s="26" t="s">
@@ -50384,10 +50377,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>203</v>
@@ -50471,10 +50464,10 @@
         <v>29</v>
       </c>
       <c r="AH1" s="2" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="AI1" s="2" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="AJ1" s="2" t="s">
         <v>30</v>
@@ -50614,15 +50607,15 @@
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="H2" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="I2">
         <v>2010</v>
@@ -50634,10 +50627,10 @@
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="P2" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="AR2">
         <v>5</v>
@@ -50654,10 +50647,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="I3">
         <v>2019</v>
@@ -50666,7 +50659,7 @@
         <v>0</v>
       </c>
       <c r="O3" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="5" spans="1:77" s="14" customFormat="1" ht="102" x14ac:dyDescent="0.2">
@@ -50680,19 +50673,19 @@
         <v>1</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="I5" s="14">
         <v>2019</v>
@@ -50707,7 +50700,7 @@
         <v>0</v>
       </c>
       <c r="Q5" s="14" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="U5" s="14">
         <v>1</v>
@@ -50743,10 +50736,10 @@
         <v>0.56599999999999995</v>
       </c>
       <c r="AF5" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="AG5" s="14" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="AJ5" s="14">
         <v>1</v>
@@ -50758,7 +50751,7 @@
         <v>320</v>
       </c>
       <c r="AM5" s="19" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="AN5" s="14">
         <v>1</v>
@@ -50779,7 +50772,7 @@
         <v>267</v>
       </c>
       <c r="BJ5" s="14" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="BK5" s="14">
         <v>0</v>
@@ -50797,7 +50790,7 @@
         <v>0</v>
       </c>
       <c r="BS5" s="14" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="BT5" s="14" t="s">
         <v>644</v>
@@ -50826,19 +50819,19 @@
         <v>1</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="I6" s="14">
         <v>2019</v>
@@ -50853,7 +50846,7 @@
         <v>0</v>
       </c>
       <c r="Q6" s="14" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="S6" s="14">
         <v>1</v>
@@ -50892,10 +50885,10 @@
         <v>0.58099999999999996</v>
       </c>
       <c r="AF6" s="14" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="AG6" s="14" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="AJ6" s="14">
         <v>1</v>
@@ -50907,7 +50900,7 @@
         <v>320</v>
       </c>
       <c r="AM6" s="19" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="AN6" s="14">
         <v>1</v>
@@ -50916,7 +50909,7 @@
         <v>724</v>
       </c>
       <c r="AP6" s="14" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="AQ6" s="14" t="s">
         <v>541</v>
@@ -50940,7 +50933,7 @@
         <v>267</v>
       </c>
       <c r="BJ6" s="14" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="BK6" s="14">
         <v>0</v>
@@ -50987,15 +50980,15 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="I7">
         <v>2009</v>
@@ -51010,10 +51003,10 @@
         <v>0</v>
       </c>
       <c r="O7" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="P7" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="U7">
         <v>1</v>
@@ -51030,16 +51023,16 @@
         <v>1</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="I8" s="14">
         <v>2006</v>
@@ -51054,10 +51047,10 @@
         <v>0</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="P8" s="14" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="U8" s="14">
         <v>1</v>
@@ -51102,7 +51095,7 @@
         <v>320</v>
       </c>
       <c r="AM8" s="14" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="AN8" s="14">
         <v>1</v>
@@ -51111,10 +51104,10 @@
         <v>724</v>
       </c>
       <c r="AP8" s="14" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="AQ8" s="14" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="BD8" s="14">
         <v>10</v>
@@ -51129,16 +51122,16 @@
         <v>267</v>
       </c>
       <c r="BJ8" s="14" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="BK8" s="14">
         <v>1</v>
       </c>
       <c r="BL8" s="14" t="s">
+        <v>809</v>
+      </c>
+      <c r="BM8" s="14" t="s">
         <v>811</v>
-      </c>
-      <c r="BM8" s="14" t="s">
-        <v>813</v>
       </c>
       <c r="BP8" s="14" t="s">
         <v>495</v>
@@ -51150,7 +51143,7 @@
         <v>2</v>
       </c>
       <c r="BS8" s="14" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="BT8" s="14" t="s">
         <v>644</v>
@@ -51162,7 +51155,7 @@
         <v>1</v>
       </c>
       <c r="BW8" s="14" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="BX8" s="14">
         <v>1</v>
@@ -51182,16 +51175,16 @@
         <v>2</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="I9" s="14">
         <v>2006</v>
@@ -51206,10 +51199,10 @@
         <v>0</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="P9" s="14" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="U9" s="14">
         <v>1</v>
@@ -51254,7 +51247,7 @@
         <v>320</v>
       </c>
       <c r="AM9" s="14" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="AN9" s="14">
         <v>1</v>
@@ -51263,10 +51256,10 @@
         <v>724</v>
       </c>
       <c r="AP9" s="14" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="AQ9" s="14" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="BD9" s="14">
         <v>10</v>
@@ -51281,16 +51274,16 @@
         <v>267</v>
       </c>
       <c r="BJ9" s="14" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="BK9" s="14">
         <v>1</v>
       </c>
       <c r="BL9" s="14" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="BM9" s="14" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="BP9" s="14" t="s">
         <v>495</v>
@@ -51302,7 +51295,7 @@
         <v>2</v>
       </c>
       <c r="BS9" s="14" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="BT9" s="14" t="s">
         <v>644</v>
@@ -51314,7 +51307,7 @@
         <v>1</v>
       </c>
       <c r="BW9" s="14" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="BX9" s="14">
         <v>1</v>
@@ -51334,16 +51327,16 @@
         <v>3</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="I10" s="14">
         <v>2006</v>
@@ -51358,10 +51351,10 @@
         <v>0</v>
       </c>
       <c r="O10" s="14" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="P10" s="14" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="U10" s="14">
         <v>1</v>
@@ -51406,7 +51399,7 @@
         <v>320</v>
       </c>
       <c r="AM10" s="14" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="AN10" s="14">
         <v>1</v>
@@ -51415,10 +51408,10 @@
         <v>724</v>
       </c>
       <c r="AP10" s="14" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="AQ10" s="14" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="BD10" s="14">
         <v>10</v>
@@ -51433,16 +51426,16 @@
         <v>267</v>
       </c>
       <c r="BJ10" s="14" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="BK10" s="14">
         <v>1</v>
       </c>
       <c r="BL10" s="14" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="BM10" s="14" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="BP10" s="14" t="s">
         <v>495</v>
@@ -51454,7 +51447,7 @@
         <v>2</v>
       </c>
       <c r="BS10" s="14" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="BT10" s="14" t="s">
         <v>644</v>
@@ -51466,7 +51459,7 @@
         <v>1</v>
       </c>
       <c r="BW10" s="14" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="BX10" s="14">
         <v>1</v>
@@ -51486,16 +51479,16 @@
         <v>4</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="I11" s="14">
         <v>2006</v>
@@ -51510,10 +51503,10 @@
         <v>0</v>
       </c>
       <c r="O11" s="14" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="P11" s="14" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="U11" s="14">
         <v>1</v>
@@ -51558,7 +51551,7 @@
         <v>320</v>
       </c>
       <c r="AM11" s="14" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="AN11" s="14">
         <v>1</v>
@@ -51567,10 +51560,10 @@
         <v>724</v>
       </c>
       <c r="AP11" s="14" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="AQ11" s="14" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="BD11" s="14">
         <v>10</v>
@@ -51585,16 +51578,16 @@
         <v>267</v>
       </c>
       <c r="BJ11" s="14" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="BK11" s="14">
         <v>1</v>
       </c>
       <c r="BL11" s="14" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="BM11" s="14" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="BP11" s="14" t="s">
         <v>495</v>
@@ -51606,7 +51599,7 @@
         <v>2</v>
       </c>
       <c r="BS11" s="14" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="BT11" s="14" t="s">
         <v>644</v>
@@ -51618,7 +51611,7 @@
         <v>1</v>
       </c>
       <c r="BW11" s="14" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="BX11" s="14">
         <v>1</v>
@@ -51638,16 +51631,16 @@
         <v>5</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="I12" s="14">
         <v>2006</v>
@@ -51662,10 +51655,10 @@
         <v>0</v>
       </c>
       <c r="O12" s="14" t="s">
+        <v>813</v>
+      </c>
+      <c r="P12" s="14" t="s">
         <v>815</v>
-      </c>
-      <c r="P12" s="14" t="s">
-        <v>817</v>
       </c>
       <c r="U12" s="14">
         <v>1</v>
@@ -51710,7 +51703,7 @@
         <v>320</v>
       </c>
       <c r="AM12" s="14" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="AN12" s="14">
         <v>1</v>
@@ -51719,10 +51712,10 @@
         <v>724</v>
       </c>
       <c r="AP12" s="14" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="AQ12" s="14" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="BD12" s="14">
         <v>10</v>
@@ -51737,16 +51730,16 @@
         <v>267</v>
       </c>
       <c r="BJ12" s="14" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="BK12" s="14">
         <v>1</v>
       </c>
       <c r="BL12" s="14" t="s">
+        <v>809</v>
+      </c>
+      <c r="BM12" s="14" t="s">
         <v>811</v>
-      </c>
-      <c r="BM12" s="14" t="s">
-        <v>813</v>
       </c>
       <c r="BP12" s="14" t="s">
         <v>495</v>
@@ -51758,7 +51751,7 @@
         <v>2</v>
       </c>
       <c r="BS12" s="14" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="BT12" s="14" t="s">
         <v>644</v>
@@ -51770,7 +51763,7 @@
         <v>1</v>
       </c>
       <c r="BW12" s="14" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="BX12" s="14">
         <v>1</v>
@@ -51790,16 +51783,16 @@
         <v>6</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="I13" s="14">
         <v>2006</v>
@@ -51814,10 +51807,10 @@
         <v>0</v>
       </c>
       <c r="O13" s="14" t="s">
+        <v>813</v>
+      </c>
+      <c r="P13" s="14" t="s">
         <v>815</v>
-      </c>
-      <c r="P13" s="14" t="s">
-        <v>817</v>
       </c>
       <c r="U13" s="14">
         <v>1</v>
@@ -51862,7 +51855,7 @@
         <v>320</v>
       </c>
       <c r="AM13" s="14" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="AN13" s="14">
         <v>1</v>
@@ -51871,10 +51864,10 @@
         <v>724</v>
       </c>
       <c r="AP13" s="14" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="AQ13" s="14" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="BD13" s="14">
         <v>10</v>
@@ -51889,16 +51882,16 @@
         <v>267</v>
       </c>
       <c r="BJ13" s="14" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="BK13" s="14">
         <v>1</v>
       </c>
       <c r="BL13" s="14" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="BM13" s="14" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="BP13" s="14" t="s">
         <v>495</v>
@@ -51910,7 +51903,7 @@
         <v>2</v>
       </c>
       <c r="BS13" s="14" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="BT13" s="14" t="s">
         <v>644</v>
@@ -51922,7 +51915,7 @@
         <v>1</v>
       </c>
       <c r="BW13" s="14" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="BX13" s="14">
         <v>1</v>
@@ -51942,16 +51935,16 @@
         <v>7</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="I14" s="14">
         <v>2006</v>
@@ -51966,10 +51959,10 @@
         <v>0</v>
       </c>
       <c r="O14" s="14" t="s">
+        <v>813</v>
+      </c>
+      <c r="P14" s="14" t="s">
         <v>815</v>
-      </c>
-      <c r="P14" s="14" t="s">
-        <v>817</v>
       </c>
       <c r="U14" s="14">
         <v>1</v>
@@ -52014,7 +52007,7 @@
         <v>320</v>
       </c>
       <c r="AM14" s="14" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="AN14" s="14">
         <v>1</v>
@@ -52023,10 +52016,10 @@
         <v>724</v>
       </c>
       <c r="AP14" s="14" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="AQ14" s="14" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="BD14" s="14">
         <v>10</v>
@@ -52041,16 +52034,16 @@
         <v>267</v>
       </c>
       <c r="BJ14" s="14" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="BK14" s="14">
         <v>1</v>
       </c>
       <c r="BL14" s="14" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="BM14" s="14" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="BP14" s="14" t="s">
         <v>495</v>
@@ -52062,7 +52055,7 @@
         <v>2</v>
       </c>
       <c r="BS14" s="14" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="BT14" s="14" t="s">
         <v>644</v>
@@ -52074,7 +52067,7 @@
         <v>1</v>
       </c>
       <c r="BW14" s="14" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="BX14" s="14">
         <v>1</v>
@@ -52094,16 +52087,16 @@
         <v>8</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="H15" s="19" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="I15" s="14">
         <v>2006</v>
@@ -52118,10 +52111,10 @@
         <v>0</v>
       </c>
       <c r="O15" s="14" t="s">
+        <v>813</v>
+      </c>
+      <c r="P15" s="14" t="s">
         <v>815</v>
-      </c>
-      <c r="P15" s="14" t="s">
-        <v>817</v>
       </c>
       <c r="U15" s="14">
         <v>1</v>
@@ -52166,7 +52159,7 @@
         <v>320</v>
       </c>
       <c r="AM15" s="14" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="AN15" s="14">
         <v>1</v>
@@ -52175,10 +52168,10 @@
         <v>724</v>
       </c>
       <c r="AP15" s="14" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="AQ15" s="14" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="BD15" s="14">
         <v>10</v>
@@ -52193,16 +52186,16 @@
         <v>267</v>
       </c>
       <c r="BJ15" s="14" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="BK15" s="14">
         <v>1</v>
       </c>
       <c r="BL15" s="14" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="BM15" s="14" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="BP15" s="14" t="s">
         <v>495</v>
@@ -52214,7 +52207,7 @@
         <v>2</v>
       </c>
       <c r="BS15" s="14" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="BT15" s="14" t="s">
         <v>644</v>
@@ -52226,7 +52219,7 @@
         <v>1</v>
       </c>
       <c r="BW15" s="14" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="BX15" s="14">
         <v>1</v>
@@ -52248,13 +52241,13 @@
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="H16" s="8" t="s">
+        <v>819</v>
+      </c>
+      <c r="P16" t="s">
         <v>821</v>
-      </c>
-      <c r="P16" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="17" spans="1:77" s="14" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -52268,16 +52261,16 @@
         <v>1</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="I17" s="14">
         <v>2012</v>
@@ -52295,7 +52288,7 @@
         <v>501</v>
       </c>
       <c r="R17" s="14" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="U17" s="14">
         <v>1</v>
@@ -52340,19 +52333,19 @@
         <v>320</v>
       </c>
       <c r="AM17" s="14" t="s">
+        <v>825</v>
+      </c>
+      <c r="AN17" s="14">
+        <v>1</v>
+      </c>
+      <c r="AO17" s="14" t="s">
+        <v>731</v>
+      </c>
+      <c r="AP17" s="14" t="s">
         <v>827</v>
       </c>
-      <c r="AN17" s="14">
-        <v>1</v>
-      </c>
-      <c r="AO17" s="14" t="s">
-        <v>732</v>
-      </c>
-      <c r="AP17" s="14" t="s">
-        <v>829</v>
-      </c>
       <c r="AQ17" s="14" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="AR17" s="14">
         <v>7</v>
@@ -52373,13 +52366,13 @@
         <v>0</v>
       </c>
       <c r="BN17" s="14" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="BO17" s="14" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="BP17" s="14" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="BQ17" s="14">
         <v>1</v>
@@ -52397,7 +52390,7 @@
         <v>1</v>
       </c>
       <c r="BW17" s="14" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="BY17" s="14" t="s">
         <v>237</v>
@@ -52414,16 +52407,16 @@
         <v>2</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="H18" s="19" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="I18" s="14">
         <v>2012</v>
@@ -52441,7 +52434,7 @@
         <v>501</v>
       </c>
       <c r="R18" s="14" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="U18" s="14">
         <v>1</v>
@@ -52486,19 +52479,19 @@
         <v>320</v>
       </c>
       <c r="AM18" s="14" t="s">
+        <v>825</v>
+      </c>
+      <c r="AN18" s="14">
+        <v>1</v>
+      </c>
+      <c r="AO18" s="14" t="s">
+        <v>731</v>
+      </c>
+      <c r="AP18" s="14" t="s">
         <v>827</v>
       </c>
-      <c r="AN18" s="14">
-        <v>1</v>
-      </c>
-      <c r="AO18" s="14" t="s">
-        <v>732</v>
-      </c>
-      <c r="AP18" s="14" t="s">
-        <v>829</v>
-      </c>
       <c r="AQ18" s="14" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="AR18" s="14">
         <v>7</v>
@@ -52519,13 +52512,13 @@
         <v>0</v>
       </c>
       <c r="BN18" s="14" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="BO18" s="14" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="BP18" s="14" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="BQ18" s="14">
         <v>1</v>
@@ -52543,7 +52536,7 @@
         <v>1</v>
       </c>
       <c r="BW18" s="14" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="BY18" s="14" t="s">
         <v>237</v>
@@ -52560,16 +52553,16 @@
         <v>3</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="H19" s="19" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="I19" s="14">
         <v>2012</v>
@@ -52584,13 +52577,13 @@
         <v>0</v>
       </c>
       <c r="O19" s="14" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="Q19" s="14" t="s">
         <v>501</v>
       </c>
       <c r="R19" s="14" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="U19" s="14">
         <v>1</v>
@@ -52617,19 +52610,19 @@
         <v>320</v>
       </c>
       <c r="AM19" s="14" t="s">
+        <v>825</v>
+      </c>
+      <c r="AN19" s="14">
+        <v>1</v>
+      </c>
+      <c r="AO19" s="14" t="s">
+        <v>731</v>
+      </c>
+      <c r="AP19" s="14" t="s">
         <v>827</v>
       </c>
-      <c r="AN19" s="14">
-        <v>1</v>
-      </c>
-      <c r="AO19" s="14" t="s">
-        <v>732</v>
-      </c>
-      <c r="AP19" s="14" t="s">
-        <v>829</v>
-      </c>
       <c r="AQ19" s="14" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="BD19" s="14">
         <v>20</v>
@@ -52647,13 +52640,13 @@
         <v>0</v>
       </c>
       <c r="BN19" s="14" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="BO19" s="14" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="BP19" s="14" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="BQ19" s="14">
         <v>1</v>
@@ -52671,7 +52664,7 @@
         <v>1</v>
       </c>
       <c r="BW19" s="14" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="BY19" s="14" t="s">
         <v>237</v>
@@ -52688,16 +52681,16 @@
         <v>4</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="I20" s="14">
         <v>2012</v>
@@ -52712,13 +52705,13 @@
         <v>0</v>
       </c>
       <c r="O20" s="14" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="Q20" s="14" t="s">
         <v>501</v>
       </c>
       <c r="R20" s="14" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="U20" s="14">
         <v>1</v>
@@ -52745,19 +52738,19 @@
         <v>320</v>
       </c>
       <c r="AM20" s="14" t="s">
+        <v>825</v>
+      </c>
+      <c r="AN20" s="14">
+        <v>1</v>
+      </c>
+      <c r="AO20" s="14" t="s">
+        <v>731</v>
+      </c>
+      <c r="AP20" s="14" t="s">
         <v>827</v>
       </c>
-      <c r="AN20" s="14">
-        <v>1</v>
-      </c>
-      <c r="AO20" s="14" t="s">
-        <v>732</v>
-      </c>
-      <c r="AP20" s="14" t="s">
-        <v>829</v>
-      </c>
       <c r="AQ20" s="14" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="BD20" s="14">
         <v>20</v>
@@ -52775,13 +52768,13 @@
         <v>0</v>
       </c>
       <c r="BN20" s="14" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="BO20" s="14" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="BP20" s="14" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="BQ20" s="14">
         <v>1</v>
@@ -52799,7 +52792,7 @@
         <v>1</v>
       </c>
       <c r="BW20" s="14" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="BY20" s="14" t="s">
         <v>237</v>
@@ -52816,15 +52809,15 @@
         <v>1</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
       <c r="G21" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="I21">
         <v>2015</v>
@@ -52839,10 +52832,10 @@
         <v>0</v>
       </c>
       <c r="O21" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="P21" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="AR21">
         <v>6</v>
@@ -52851,10 +52844,10 @@
         <v>1</v>
       </c>
       <c r="BL21" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="BM21" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
     </row>
     <row r="22" spans="1:77" ht="34" x14ac:dyDescent="0.2">
@@ -52868,15 +52861,15 @@
         <v>1</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
       <c r="G22" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="I22">
         <v>2017</v>
@@ -52891,7 +52884,7 @@
         <v>0</v>
       </c>
       <c r="O22" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
     </row>
     <row r="23" spans="1:77" ht="153" x14ac:dyDescent="0.2">
@@ -52905,15 +52898,15 @@
         <v>1</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="E23" s="16"/>
       <c r="F23" s="16"/>
       <c r="G23" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="I23">
         <v>2013</v>
@@ -52928,7 +52921,7 @@
         <v>0</v>
       </c>
       <c r="O23" s="8" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="24" spans="1:77" ht="68" x14ac:dyDescent="0.2">
@@ -52944,10 +52937,10 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="I24">
         <v>2015</v>
@@ -52962,10 +52955,10 @@
         <v>0</v>
       </c>
       <c r="O24" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="P24" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="25" spans="1:77" s="14" customFormat="1" ht="119" x14ac:dyDescent="0.2">
@@ -52979,16 +52972,16 @@
         <v>1</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="H25" s="19" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="I25" s="14">
         <v>2009</v>
@@ -53003,7 +52996,7 @@
         <v>0</v>
       </c>
       <c r="P25" s="14" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="Y25" s="14">
         <v>254</v>
@@ -53027,19 +53020,19 @@
         <v>320</v>
       </c>
       <c r="AM25" s="19" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="AN25" s="14">
         <v>1</v>
       </c>
       <c r="AO25" s="14" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="AP25" s="14" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="AQ25" s="14" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="AS25" s="14">
         <v>0.94499999999999995</v>
@@ -53066,7 +53059,7 @@
         <v>0</v>
       </c>
       <c r="BJ25" s="14" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="BK25" s="14">
         <v>0</v>
@@ -53075,7 +53068,7 @@
         <v>251</v>
       </c>
       <c r="BP25" s="14" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="BQ25" s="14">
         <v>1</v>
@@ -53090,7 +53083,7 @@
         <v>2</v>
       </c>
       <c r="BV25" s="14" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="BW25" s="14" t="s">
         <v>691</v>
@@ -53113,10 +53106,10 @@
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="I26">
         <v>2014</v>
@@ -53131,7 +53124,7 @@
         <v>0</v>
       </c>
       <c r="O26" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="27" spans="1:77" ht="68" x14ac:dyDescent="0.2">
@@ -53145,10 +53138,10 @@
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="I27">
         <v>2016</v>
@@ -53163,7 +53156,7 @@
         <v>1</v>
       </c>
       <c r="O27" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
     <row r="28" spans="1:77" ht="51" x14ac:dyDescent="0.2">
@@ -53177,10 +53170,10 @@
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="I28">
         <v>2014</v>
@@ -53195,7 +53188,7 @@
         <v>1</v>
       </c>
       <c r="P28" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
     </row>
     <row r="29" spans="1:77" x14ac:dyDescent="0.2">
@@ -53209,10 +53202,10 @@
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="H29" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="I29">
         <v>2015</v>
@@ -53221,10 +53214,10 @@
         <v>0</v>
       </c>
       <c r="O29" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="P29" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
   </sheetData>

</xml_diff>